<commit_message>
config and excel update for master
</commit_message>
<xml_diff>
--- a/src/test/java/countries.xlsx
+++ b/src/test/java/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dededim\dene\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60BB18E-6AA8-42EB-8450-371C1376B083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736BBD3B-C257-41E2-879B-847C18768734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     <t>Moscow</t>
   </si>
   <si>
-    <t>Develop  from</t>
+    <t>master  from</t>
   </si>
 </sst>
 </file>

</xml_diff>